<commit_message>
Update IP - EX 25 - Formatacao condicional com formulas (Anexo).xlsx
Exercicio
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 25 - Formatacao condicional com formulas (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 25 - Formatacao condicional com formulas (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C808305-7D1F-495E-B371-022C97DBCD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D0E04E-8E48-4D86-A680-E07E1BE04D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
@@ -131,7 +153,7 @@
     <t>"A utilização de formatação condicional através de fórmulas permite a formatação tanto de células, linhas/colunas inteiras fazendo referência a uma outra célula."</t>
   </si>
   <si>
-    <t>TOMAR CUIDADO COM O  _____________  ___  __________ .</t>
+    <t>TOMAR CUIDADO COM O TRAVAMENTO DAS CÉLULAS .</t>
   </si>
 </sst>
 </file>
@@ -626,8 +648,56 @@
     <cellStyle name="SAPBEXfilterDrill" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Vírgula 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1130,7 +1200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1317,7 +1387,7 @@
   <dimension ref="B1:Q17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,6 +1689,14 @@
     <mergeCell ref="B2:Q6"/>
     <mergeCell ref="G13:K15"/>
   </mergeCells>
+  <conditionalFormatting sqref="B9:E17">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>IF($E9="aprovado",1,0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>IF($E9="reprovado",1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1628,14 +1706,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1679,10 +1758,16 @@
       <c r="D4" s="22">
         <v>8</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="23">
+        <f>(C4+(D4*2))/2</f>
+        <v>9.5</v>
+      </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
+      <c r="H4" s="22" t="str" cm="1">
+        <f t="array" ref="H4">_xlfn.IFS(E4&gt;=6,"Aprovado",G4&gt;=5,"Aprovado",G4&lt;5,"Reprovado")</f>
+        <v>Aprovado</v>
+      </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1693,14 +1778,23 @@
         <v>2</v>
       </c>
       <c r="D5" s="22">
+        <v>4</v>
+      </c>
+      <c r="E5" s="23">
+        <f t="shared" ref="E5:E8" si="0">(C5+(D5*2))/2</f>
         <v>5</v>
       </c>
-      <c r="E5" s="23"/>
       <c r="F5" s="22">
         <v>6</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
+      <c r="G5" s="22">
+        <f>(E5+F5)/2</f>
+        <v>5.5</v>
+      </c>
+      <c r="H5" s="22" t="str" cm="1">
+        <f t="array" ref="H5">_xlfn.IFS(E5&gt;=6,"Aprovado",G5&gt;=5,"Aprovado",G5&lt;5,"Reprovado")</f>
+        <v>Aprovado</v>
+      </c>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1713,10 +1807,16 @@
       <c r="D6" s="22">
         <v>6</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="23">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
+      <c r="H6" s="22" t="str" cm="1">
+        <f t="array" ref="H6">_xlfn.IFS(E6&gt;=6,"Aprovado",G6&gt;=5,"Aprovado",G6&lt;5,"Reprovado")</f>
+        <v>Aprovado</v>
+      </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -1729,10 +1829,16 @@
       <c r="D7" s="22">
         <v>7</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="23">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
+      <c r="H7" s="22" t="str" cm="1">
+        <f t="array" ref="H7">_xlfn.IFS(E7&gt;=6,"Aprovado",G7&gt;=5,"Aprovado",G7&lt;5,"Reprovado")</f>
+        <v>Aprovado</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
@@ -1742,14 +1848,23 @@
         <v>2</v>
       </c>
       <c r="D8" s="22">
+        <v>3</v>
+      </c>
+      <c r="E8" s="23">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E8" s="23"/>
       <c r="F8" s="22">
         <v>4</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="G8" s="22">
+        <f>(E8+F8)/2</f>
+        <v>4</v>
+      </c>
+      <c r="H8" s="22" t="str" cm="1">
+        <f t="array" ref="H8">_xlfn.IFS(E8&gt;=6,"Aprovado",G8&gt;=5,"Aprovado",G8&lt;5,"Reprovado")</f>
+        <v>Reprovado</v>
+      </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1820,6 +1935,14 @@
   <mergeCells count="1">
     <mergeCell ref="B15:E18"/>
   </mergeCells>
+  <conditionalFormatting sqref="B4:H8">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>IF($H4="aprovado",1,0)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>IF($H4="reprovado",1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>